<commit_message>
all updates to include tri proximity tables
</commit_message>
<xml_diff>
--- a/data/hfc_facilities-4-8-22_w_additions V2_frsID.xlsx
+++ b/data/hfc_facilities-4-8-22_w_additions V2_frsID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\Git Repos\F_Gas_Rules\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AA99E4-0C07-4AE2-97B1-D72BECD0A7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95495B12-0A24-4E43-A75C-EF28DE10E166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1950" windowWidth="28770" windowHeight="11745" xr2:uid="{B999005D-378C-4D50-B09E-E8C4AF2F8FB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B999005D-378C-4D50-B09E-E8C4AF2F8FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t>Chemical</t>
   </si>
@@ -277,6 +277,45 @@
   </si>
   <si>
     <t>IN</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>A-GAS</t>
+  </si>
+  <si>
+    <t>AEROPRES-SANDIMAS</t>
+  </si>
+  <si>
+    <t>CFI-PortNeal</t>
+  </si>
+  <si>
+    <t>Linde-Whiting</t>
+  </si>
+  <si>
+    <t>APC-Geismar</t>
+  </si>
+  <si>
+    <t>HaltermanCarless</t>
+  </si>
+  <si>
+    <t>APC-PortAuthur</t>
+  </si>
+  <si>
+    <t>DiversifiedG&amp;O</t>
+  </si>
+  <si>
+    <t>Linde-Decatur</t>
+  </si>
+  <si>
+    <t>Diversified-CPC</t>
+  </si>
+  <si>
+    <t>AEROPRES-SIBLEY</t>
+  </si>
+  <si>
+    <t>Chemours-CorpusChristie</t>
   </si>
 </sst>
 </file>
@@ -365,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -431,6 +470,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{636D6C34-0F1C-40B4-9259-5B7701D238C2}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,13 +798,14 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="15"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="15"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -773,46 +816,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -823,40 +869,43 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>71730</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>33.116667</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-92.680555999999996</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>106401</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>99143</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1003890</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>110033515540</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>325120</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -867,28 +916,31 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>91773</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>34.101469999999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-117.81204</v>
       </c>
-      <c r="O3" s="24">
+      <c r="P3" s="24">
         <v>110000514122</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -899,43 +951,46 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>51054</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>42.327860000000001</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>-96.364890000000003</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2888938</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>389421</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1006005</v>
       </c>
-      <c r="O4" s="4">
+      <c r="P4" s="4">
         <v>110000414089</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>325311</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -946,43 +1001,46 @@
         <v>58</v>
       </c>
       <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>46312</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>41.668630999999998</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-87.472829000000004</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>183562</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>2</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>1002119</v>
       </c>
-      <c r="O5" s="4">
+      <c r="P5" s="4">
         <v>110002321381</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>325120</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -993,43 +1051,46 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="F6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>70734</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>30.183807999999999</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>-90.9876</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>56325</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>1002698</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="4">
         <v>110006020304</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>325120</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1040,28 +1101,31 @@
         <v>47</v>
       </c>
       <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>77578</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>29.45636</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>-95.32526</v>
       </c>
-      <c r="O7" s="25">
+      <c r="P7" s="25">
         <v>110000599479</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1072,43 +1136,46 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="F8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>77640</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>29.859444</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>-93.965833000000003</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2423361</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>673</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>1006402</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <v>110043802819</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>325120</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1119,28 +1186,31 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>25201</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>38.2951422245565</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-81.4628883715081</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>110069506877</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1150,35 +1220,38 @@
       <c r="C10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="F10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>35601</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>34.643332999999998</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="5">
         <v>-87.065832999999998</v>
       </c>
-      <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="26" t="s">
+      <c r="O10" s="7"/>
+      <c r="P10" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1189,29 +1262,32 @@
         <v>62</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="F11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>95203</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>37.948689999999999</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>-121.32605599999999</v>
       </c>
-      <c r="O11" s="27" t="s">
+      <c r="P11" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1222,34 +1298,37 @@
         <v>35</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="F12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <v>60410</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>41.411985000000001</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>-88.202211000000005</v>
       </c>
-      <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="25">
+      <c r="O12" s="7"/>
+      <c r="P12" s="25">
         <v>110000578214</v>
       </c>
-      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1260,29 +1339,32 @@
         <v>72</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <v>71073</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>32.409059999999997</v>
       </c>
-      <c r="J13" s="5">
+      <c r="K13" s="5">
         <v>-93.282629999999997</v>
       </c>
-      <c r="O13" s="25">
+      <c r="P13" s="25">
         <v>110008381438</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1292,41 +1374,44 @@
       <c r="C14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="F14" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="H14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>78359</v>
       </c>
-      <c r="I14" s="5">
+      <c r="J14" s="5">
         <v>27.881388999999999</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>-97.252222000000003</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>26401</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>14848</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>1006314</v>
       </c>
-      <c r="O14" s="4">
+      <c r="P14" s="4">
         <v>110000746532</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>325120</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -1336,38 +1421,41 @@
       <c r="C15" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="H15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>70734</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="5">
         <v>30.225277999999999</v>
       </c>
-      <c r="J15" s="5">
+      <c r="K15" s="5">
         <v>-91.052499999999995</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>528957</v>
       </c>
-      <c r="L15" s="5">
+      <c r="M15" s="5">
         <v>423328</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5">
         <v>1006070</v>
       </c>
-      <c r="O15" s="8">
+      <c r="P15" s="8">
         <v>110033659878</v>
       </c>
-      <c r="P15" s="5">
+      <c r="Q15" s="5">
         <v>325120</v>
       </c>
     </row>

</xml_diff>